<commit_message>
update API Interface Upload & UI Code Add Device
</commit_message>
<xml_diff>
--- a/src/main/resources/template/ExportIntetface.xlsx
+++ b/src/main/resources/template/ExportIntetface.xlsx
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:O22"/>
 </workbook>
 </file>
 
@@ -33,7 +32,33 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>所属项目(ID)</t>
+    <r>
+      <t>所属项目(格式：</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>项目名称(项目ID)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -41,7 +66,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +86,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -399,7 +433,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="34.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="27.625" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.75" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.625" style="2" customWidth="1"/>
@@ -426,14 +460,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C1048576">
       <formula1>"GET,POST"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1 A1"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
-      <formula1>"App(1)"</formula1>
-    </dataValidation>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="C1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>